<commit_message>
added an Excel with the results for the  third part of the experiments
</commit_message>
<xml_diff>
--- a/evaluation/group_size_to_duration.xlsx
+++ b/evaluation/group_size_to_duration.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yonik\grouped_sampling\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{38E109EA-CE79-4634-A94E-29CBCCF29496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A1881C-8A49-4060-B3CC-7B81B1D7F2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="group_size_to_duration" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>duration in hours</t>
   </si>
@@ -29,18 +40,6 @@
   </si>
   <si>
     <t>duration seconds</t>
-  </si>
-  <si>
-    <t>סכום</t>
-  </si>
-  <si>
-    <t>ממוצע</t>
-  </si>
-  <si>
-    <t>סכום מצטבר</t>
-  </si>
-  <si>
-    <t>ספירה</t>
   </si>
   <si>
     <t>BERT_f1</t>
@@ -67,18 +66,21 @@
     <t>זמן ריצה בשניות</t>
   </si>
   <si>
-    <t>אלגוריתמים קיימים (גודל קבוצה=1)</t>
+    <t>דגימה בקבוצות</t>
   </si>
   <si>
-    <t>דגימה בקבוצות (גודל קבוצה =2048)</t>
+    <t>האלגוריתם האוטו-ריגרסיבי</t>
+  </si>
+  <si>
+    <t>האלגוריתם                         האוטו-ריגרסיבי</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -558,10 +560,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - הדגשה1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1088,7 +1091,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1101,17 +1104,40 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="he-IL" sz="2800"/>
-              <a:t>תרשים ב - מדדי </a:t>
+              <a:rPr lang="he-IL" sz="2800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>מדדי</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2800"/>
+              <a:rPr lang="en-US" sz="2800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
               <a:t>BERT </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="he-IL" sz="2800"/>
-              <a:t>ממוצעים</a:t>
+              <a:rPr lang="he-IL" sz="2800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> כפונקציה של גודל הקבוצה</a:t>
             </a:r>
+            <a:endParaRPr lang="he-IL" sz="2800">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2800"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="he-IL" sz="2800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>מדדים גבוהים = הצלחה גדולה יותר</a:t>
+            </a:r>
+            <a:endParaRPr lang="he-IL" sz="2800">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1128,7 +1154,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1160,7 +1186,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>אלגוריתמים קיימים (גודל קבוצה=1)</c:v>
+                  <c:v>האלגוריתם האוטו-ריגרסיבי</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1190,7 +1216,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1283,7 +1309,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>דגימה בקבוצות (גודל קבוצה =2048)</c:v>
+                  <c:v>דגימה בקבוצות</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1313,7 +1339,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1541,7 +1567,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1628,8 +1654,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="he-IL" sz="2800"/>
-              <a:t>תרשים א - זמן ריצה בשעות</a:t>
+              <a:rPr lang="he-IL" sz="2800" b="0"/>
+              <a:t>זמן ריצה בשעות כפונקציה של גודל הקבוצה </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1695,6 +1721,39 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BE9513FE-F97F-4AB5-A4B0-5D3AF74415D4}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[ערך]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="he-IL"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-BF76-4A3D-AFCE-BA23199B75BA}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1709,7 +1768,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1758,10 +1817,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>אלגוריתמים קיימים (גודל קבוצה=1)</c:v>
+                  <c:v>האלגוריתם                         האוטו-ריגרסיבי</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>דגימה בקבוצות (גודל קבוצה =2048)</c:v>
+                  <c:v>דגימה בקבוצות</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1772,8 +1831,8 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>33.049233746859699</c:v>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.7952455547120801E-2</c:v>
@@ -1830,7 +1889,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1873,7 +1932,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3671,14 +3730,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>72572</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>662214</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>82550</xdr:colOff>
+      <xdr:colOff>82551</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>136071</xdr:rowOff>
     </xdr:to>
@@ -4004,11 +4063,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4024,7 +4083,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4036,13 +4095,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -4354,34 +4413,34 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2">
-        <v>33.049233746859699</v>
+        <v>13</v>
+      </c>
+      <c r="B19" s="3">
+        <v>33</v>
       </c>
       <c r="C19">
         <f>60*B19</f>
-        <v>1982.9540248115818</v>
+        <v>1980</v>
       </c>
       <c r="D19">
         <f>C19*60</f>
-        <v>118977.24148869491</v>
+        <v>118800</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B20" s="2">
         <v>2.7952455547120801E-2</v>
@@ -4397,28 +4456,28 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1">
         <f>B19/B20-1</f>
-        <v>1181.3374047101877</v>
+        <v>1179.5760658261422</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B23">
         <v>0.65300000000000002</v>
@@ -4432,7 +4491,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B24">
         <v>0.747</v>
@@ -4446,7 +4505,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1">
         <f>(B24/B23)-1</f>
@@ -4463,6 +4522,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>